<commit_message>
Fix bug in a_psat study_utils.py
</commit_message>
<xml_diff>
--- a/a_psat/data/study_curriculum_data.xlsx
+++ b/a_psat/data/study_curriculum_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\paedison3\a_psat\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_psat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB728130-3053-46FD-A90C-2E7AD7C2A3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F8B3FB-EBC0-49B5-AB05-3E499EE30E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="600" windowWidth="12600" windowHeight="15150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="9" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="399">
   <si>
     <t>year</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1182,6 +1182,121 @@
   </si>
   <si>
     <t>최민지</t>
+  </si>
+  <si>
+    <t>PSAT탐구1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>이은비</t>
+  </si>
+  <si>
+    <t>이현정</t>
+  </si>
+  <si>
+    <t>강석헌</t>
+  </si>
+  <si>
+    <t>황준석</t>
+  </si>
+  <si>
+    <t>강인성</t>
+  </si>
+  <si>
+    <t>김광일</t>
+  </si>
+  <si>
+    <t>박윤재</t>
+  </si>
+  <si>
+    <t>이제유</t>
+  </si>
+  <si>
+    <t>문소윤</t>
+  </si>
+  <si>
+    <t>이응범</t>
+  </si>
+  <si>
+    <t>나연재</t>
+  </si>
+  <si>
+    <t>서유림</t>
+  </si>
+  <si>
+    <t>최윤희</t>
+  </si>
+  <si>
+    <t>황명하</t>
+  </si>
+  <si>
+    <t>강호경</t>
+  </si>
+  <si>
+    <t>안홍진</t>
+  </si>
+  <si>
+    <t>하다현</t>
+  </si>
+  <si>
+    <t>공현우</t>
+  </si>
+  <si>
+    <t>김나령</t>
+  </si>
+  <si>
+    <t>김연주</t>
+  </si>
+  <si>
+    <t>김유정</t>
+  </si>
+  <si>
+    <t>김효인</t>
+  </si>
+  <si>
+    <t>이윤정</t>
+  </si>
+  <si>
+    <t>지명원</t>
+  </si>
+  <si>
+    <t>김성진</t>
+  </si>
+  <si>
+    <t>안지현</t>
+  </si>
+  <si>
+    <t>우유민</t>
+  </si>
+  <si>
+    <t>이지석</t>
+  </si>
+  <si>
+    <t>정희성</t>
+  </si>
+  <si>
+    <t>추현우</t>
+  </si>
+  <si>
+    <t>김다현</t>
+  </si>
+  <si>
+    <t>이송윤</t>
+  </si>
+  <si>
+    <t>고민정</t>
+  </si>
+  <si>
+    <t>서현석</t>
+  </si>
+  <si>
+    <t>박소현</t>
+  </si>
+  <si>
+    <t>양청주</t>
+  </si>
+  <si>
+    <t>최지율</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1652,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1642,11 +1757,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD90C9E2-0442-4F0C-8721-2DB5A704E182}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2118,6 +2233,60 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>2025</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>361</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" cm="1">
+        <f t="array" ref="H18">_xlfn._xlws.FILTER(category!A:A,(category!B:B=curriculum!F18)*(category!C:C=curriculum!G18))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2025</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" cm="1">
+        <f t="array" ref="H19">_xlfn._xlws.FILTER(category!A:A,(category!B:B=curriculum!F19)*(category!C:C=curriculum!G19))</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H17" xr:uid="{CD90C9E2-0442-4F0C-8721-2DB5A704E182}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
@@ -2131,11 +2300,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G421"/>
+  <dimension ref="A1:G435"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A326" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F343" sqref="F343"/>
+      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E391" sqref="E391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2174,7 +2343,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" cm="1">
-        <f t="array" ref="A2:A373">_xlfn.SEQUENCE(COUNT(B:B))</f>
+        <f t="array" ref="A2:A435">_xlfn.SEQUENCE(COUNT(B:B))</f>
         <v>1</v>
       </c>
       <c r="B2">
@@ -11102,148 +11271,1492 @@
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E374"/>
+      <c r="A374">
+        <v>373</v>
+      </c>
+      <c r="B374">
+        <v>2025</v>
+      </c>
+      <c r="C374">
+        <v>2</v>
+      </c>
+      <c r="D374" t="s">
+        <v>90</v>
+      </c>
+      <c r="E374">
+        <v>17101038</v>
+      </c>
+      <c r="F374" t="s">
+        <v>330</v>
+      </c>
+      <c r="G374" cm="1">
+        <f t="array" ref="G374">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B374)*(curriculum!C:C=C374)*(curriculum!D:D=D374))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E375"/>
+      <c r="A375">
+        <v>374</v>
+      </c>
+      <c r="B375">
+        <v>2025</v>
+      </c>
+      <c r="C375">
+        <v>2</v>
+      </c>
+      <c r="D375" t="s">
+        <v>90</v>
+      </c>
+      <c r="E375">
+        <v>20100406</v>
+      </c>
+      <c r="F375" t="s">
+        <v>332</v>
+      </c>
+      <c r="G375" cm="1">
+        <f t="array" ref="G375">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B375)*(curriculum!C:C=C375)*(curriculum!D:D=D375))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E376"/>
+      <c r="A376">
+        <v>375</v>
+      </c>
+      <c r="B376">
+        <v>2025</v>
+      </c>
+      <c r="C376">
+        <v>2</v>
+      </c>
+      <c r="D376" t="s">
+        <v>90</v>
+      </c>
+      <c r="E376">
+        <v>20101061</v>
+      </c>
+      <c r="F376" t="s">
+        <v>362</v>
+      </c>
+      <c r="G376" cm="1">
+        <f t="array" ref="G376">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B376)*(curriculum!C:C=C376)*(curriculum!D:D=D376))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E377"/>
+      <c r="A377">
+        <v>376</v>
+      </c>
+      <c r="B377">
+        <v>2025</v>
+      </c>
+      <c r="C377">
+        <v>2</v>
+      </c>
+      <c r="D377" t="s">
+        <v>90</v>
+      </c>
+      <c r="E377">
+        <v>20101126</v>
+      </c>
+      <c r="F377" t="s">
+        <v>363</v>
+      </c>
+      <c r="G377" cm="1">
+        <f t="array" ref="G377">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B377)*(curriculum!C:C=C377)*(curriculum!D:D=D377))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E378"/>
+      <c r="A378">
+        <v>377</v>
+      </c>
+      <c r="B378">
+        <v>2025</v>
+      </c>
+      <c r="C378">
+        <v>2</v>
+      </c>
+      <c r="D378" t="s">
+        <v>90</v>
+      </c>
+      <c r="E378">
+        <v>20101149</v>
+      </c>
+      <c r="F378" t="s">
+        <v>364</v>
+      </c>
+      <c r="G378" cm="1">
+        <f t="array" ref="G378">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B378)*(curriculum!C:C=C378)*(curriculum!D:D=D378))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E379"/>
+      <c r="A379">
+        <v>378</v>
+      </c>
+      <c r="B379">
+        <v>2025</v>
+      </c>
+      <c r="C379">
+        <v>2</v>
+      </c>
+      <c r="D379" t="s">
+        <v>90</v>
+      </c>
+      <c r="E379">
+        <v>21101073</v>
+      </c>
+      <c r="F379" t="s">
+        <v>197</v>
+      </c>
+      <c r="G379" cm="1">
+        <f t="array" ref="G379">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B379)*(curriculum!C:C=C379)*(curriculum!D:D=D379))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E380"/>
+      <c r="A380">
+        <v>379</v>
+      </c>
+      <c r="B380">
+        <v>2025</v>
+      </c>
+      <c r="C380">
+        <v>2</v>
+      </c>
+      <c r="D380" t="s">
+        <v>90</v>
+      </c>
+      <c r="E380">
+        <v>21101117</v>
+      </c>
+      <c r="F380" t="s">
+        <v>365</v>
+      </c>
+      <c r="G380" cm="1">
+        <f t="array" ref="G380">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B380)*(curriculum!C:C=C380)*(curriculum!D:D=D380))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E381"/>
+      <c r="A381">
+        <v>380</v>
+      </c>
+      <c r="B381">
+        <v>2025</v>
+      </c>
+      <c r="C381">
+        <v>2</v>
+      </c>
+      <c r="D381" t="s">
+        <v>90</v>
+      </c>
+      <c r="E381">
+        <v>21101389</v>
+      </c>
+      <c r="F381" t="s">
+        <v>366</v>
+      </c>
+      <c r="G381" cm="1">
+        <f t="array" ref="G381">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B381)*(curriculum!C:C=C381)*(curriculum!D:D=D381))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E382"/>
+      <c r="A382">
+        <v>381</v>
+      </c>
+      <c r="B382">
+        <v>2025</v>
+      </c>
+      <c r="C382">
+        <v>2</v>
+      </c>
+      <c r="D382" t="s">
+        <v>90</v>
+      </c>
+      <c r="E382">
+        <v>21102347</v>
+      </c>
+      <c r="F382" t="s">
+        <v>367</v>
+      </c>
+      <c r="G382" cm="1">
+        <f t="array" ref="G382">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B382)*(curriculum!C:C=C382)*(curriculum!D:D=D382))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E383"/>
+      <c r="A383">
+        <v>382</v>
+      </c>
+      <c r="B383">
+        <v>2025</v>
+      </c>
+      <c r="C383">
+        <v>2</v>
+      </c>
+      <c r="D383" t="s">
+        <v>90</v>
+      </c>
+      <c r="E383">
+        <v>22101075</v>
+      </c>
+      <c r="F383" t="s">
+        <v>368</v>
+      </c>
+      <c r="G383" cm="1">
+        <f t="array" ref="G383">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B383)*(curriculum!C:C=C383)*(curriculum!D:D=D383))</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E384"/>
-    </row>
-    <row r="385" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E385"/>
-    </row>
-    <row r="386" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E386"/>
-    </row>
-    <row r="387" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E387"/>
-    </row>
-    <row r="388" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E388"/>
-    </row>
-    <row r="389" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E389"/>
-    </row>
-    <row r="390" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E390"/>
-    </row>
-    <row r="391" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E391"/>
-    </row>
-    <row r="392" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E392"/>
-    </row>
-    <row r="393" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E393"/>
-    </row>
-    <row r="394" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E394"/>
-    </row>
-    <row r="395" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E395"/>
-    </row>
-    <row r="396" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E396"/>
-    </row>
-    <row r="397" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E397"/>
-    </row>
-    <row r="398" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E398"/>
-    </row>
-    <row r="399" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E399"/>
-    </row>
-    <row r="400" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E400"/>
-    </row>
-    <row r="401" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E401"/>
-    </row>
-    <row r="402" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E402"/>
-    </row>
-    <row r="403" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E403"/>
-    </row>
-    <row r="404" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E404"/>
-    </row>
-    <row r="405" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E405"/>
-    </row>
-    <row r="406" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E406"/>
-    </row>
-    <row r="407" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E407"/>
-    </row>
-    <row r="408" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E408"/>
-    </row>
-    <row r="409" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E409"/>
-    </row>
-    <row r="410" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E410"/>
-    </row>
-    <row r="411" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E411"/>
-    </row>
-    <row r="412" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E412"/>
-    </row>
-    <row r="413" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E413"/>
-    </row>
-    <row r="414" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E414"/>
-    </row>
-    <row r="415" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E415"/>
-    </row>
-    <row r="416" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E416"/>
-    </row>
-    <row r="417" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E417"/>
-    </row>
-    <row r="418" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E418"/>
-    </row>
-    <row r="419" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E419"/>
-    </row>
-    <row r="420" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E420"/>
-    </row>
-    <row r="421" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E421"/>
+      <c r="A384">
+        <v>383</v>
+      </c>
+      <c r="B384">
+        <v>2025</v>
+      </c>
+      <c r="C384">
+        <v>2</v>
+      </c>
+      <c r="D384" t="s">
+        <v>90</v>
+      </c>
+      <c r="E384">
+        <v>22101090</v>
+      </c>
+      <c r="F384" t="s">
+        <v>369</v>
+      </c>
+      <c r="G384" cm="1">
+        <f t="array" ref="G384">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B384)*(curriculum!C:C=C384)*(curriculum!D:D=D384))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A385">
+        <v>384</v>
+      </c>
+      <c r="B385">
+        <v>2025</v>
+      </c>
+      <c r="C385">
+        <v>2</v>
+      </c>
+      <c r="D385" t="s">
+        <v>90</v>
+      </c>
+      <c r="E385">
+        <v>23101075</v>
+      </c>
+      <c r="F385" t="s">
+        <v>370</v>
+      </c>
+      <c r="G385" cm="1">
+        <f t="array" ref="G385">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B385)*(curriculum!C:C=C385)*(curriculum!D:D=D385))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A386">
+        <v>385</v>
+      </c>
+      <c r="B386">
+        <v>2025</v>
+      </c>
+      <c r="C386">
+        <v>2</v>
+      </c>
+      <c r="D386" t="s">
+        <v>90</v>
+      </c>
+      <c r="E386">
+        <v>23101094</v>
+      </c>
+      <c r="F386" t="s">
+        <v>371</v>
+      </c>
+      <c r="G386" cm="1">
+        <f t="array" ref="G386">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B386)*(curriculum!C:C=C386)*(curriculum!D:D=D386))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A387">
+        <v>386</v>
+      </c>
+      <c r="B387">
+        <v>2025</v>
+      </c>
+      <c r="C387">
+        <v>2</v>
+      </c>
+      <c r="D387" t="s">
+        <v>90</v>
+      </c>
+      <c r="E387">
+        <v>23101102</v>
+      </c>
+      <c r="F387" t="s">
+        <v>222</v>
+      </c>
+      <c r="G387" cm="1">
+        <f t="array" ref="G387">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B387)*(curriculum!C:C=C387)*(curriculum!D:D=D387))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A388">
+        <v>387</v>
+      </c>
+      <c r="B388">
+        <v>2025</v>
+      </c>
+      <c r="C388">
+        <v>2</v>
+      </c>
+      <c r="D388" t="s">
+        <v>90</v>
+      </c>
+      <c r="E388">
+        <v>24101099</v>
+      </c>
+      <c r="F388" t="s">
+        <v>372</v>
+      </c>
+      <c r="G388" cm="1">
+        <f t="array" ref="G388">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B388)*(curriculum!C:C=C388)*(curriculum!D:D=D388))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A389">
+        <v>388</v>
+      </c>
+      <c r="B389">
+        <v>2025</v>
+      </c>
+      <c r="C389">
+        <v>2</v>
+      </c>
+      <c r="D389" t="s">
+        <v>90</v>
+      </c>
+      <c r="E389">
+        <v>24101102</v>
+      </c>
+      <c r="F389" t="s">
+        <v>373</v>
+      </c>
+      <c r="G389" cm="1">
+        <f t="array" ref="G389">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B389)*(curriculum!C:C=C389)*(curriculum!D:D=D389))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A390">
+        <v>389</v>
+      </c>
+      <c r="B390">
+        <v>2025</v>
+      </c>
+      <c r="C390">
+        <v>2</v>
+      </c>
+      <c r="D390" t="s">
+        <v>90</v>
+      </c>
+      <c r="E390">
+        <v>24101132</v>
+      </c>
+      <c r="F390" t="s">
+        <v>374</v>
+      </c>
+      <c r="G390" cm="1">
+        <f t="array" ref="G390">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B390)*(curriculum!C:C=C390)*(curriculum!D:D=D390))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A391">
+        <v>390</v>
+      </c>
+      <c r="B391">
+        <v>2025</v>
+      </c>
+      <c r="C391">
+        <v>2</v>
+      </c>
+      <c r="D391" t="s">
+        <v>91</v>
+      </c>
+      <c r="E391">
+        <v>201803958</v>
+      </c>
+      <c r="F391" t="s">
+        <v>375</v>
+      </c>
+      <c r="G391" cm="1">
+        <f t="array" ref="G391">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B391)*(curriculum!C:C=C391)*(curriculum!D:D=D391))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A392">
+        <v>391</v>
+      </c>
+      <c r="B392">
+        <v>2025</v>
+      </c>
+      <c r="C392">
+        <v>2</v>
+      </c>
+      <c r="D392" t="s">
+        <v>91</v>
+      </c>
+      <c r="E392">
+        <v>201900361</v>
+      </c>
+      <c r="F392" t="s">
+        <v>376</v>
+      </c>
+      <c r="G392" cm="1">
+        <f t="array" ref="G392">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B392)*(curriculum!C:C=C392)*(curriculum!D:D=D392))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A393">
+        <v>392</v>
+      </c>
+      <c r="B393">
+        <v>2025</v>
+      </c>
+      <c r="C393">
+        <v>2</v>
+      </c>
+      <c r="D393" t="s">
+        <v>91</v>
+      </c>
+      <c r="E393">
+        <v>201902123</v>
+      </c>
+      <c r="F393" t="s">
+        <v>377</v>
+      </c>
+      <c r="G393" cm="1">
+        <f t="array" ref="G393">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B393)*(curriculum!C:C=C393)*(curriculum!D:D=D393))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A394">
+        <v>393</v>
+      </c>
+      <c r="B394">
+        <v>2025</v>
+      </c>
+      <c r="C394">
+        <v>2</v>
+      </c>
+      <c r="D394" t="s">
+        <v>91</v>
+      </c>
+      <c r="E394">
+        <v>201903711</v>
+      </c>
+      <c r="F394" t="s">
+        <v>378</v>
+      </c>
+      <c r="G394" cm="1">
+        <f t="array" ref="G394">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B394)*(curriculum!C:C=C394)*(curriculum!D:D=D394))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A395">
+        <v>394</v>
+      </c>
+      <c r="B395">
+        <v>2025</v>
+      </c>
+      <c r="C395">
+        <v>2</v>
+      </c>
+      <c r="D395" t="s">
+        <v>91</v>
+      </c>
+      <c r="E395">
+        <v>202000274</v>
+      </c>
+      <c r="F395" t="s">
+        <v>379</v>
+      </c>
+      <c r="G395" cm="1">
+        <f t="array" ref="G395">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B395)*(curriculum!C:C=C395)*(curriculum!D:D=D395))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A396">
+        <v>395</v>
+      </c>
+      <c r="B396">
+        <v>2025</v>
+      </c>
+      <c r="C396">
+        <v>2</v>
+      </c>
+      <c r="D396" t="s">
+        <v>91</v>
+      </c>
+      <c r="E396">
+        <v>202002584</v>
+      </c>
+      <c r="F396" t="s">
+        <v>341</v>
+      </c>
+      <c r="G396" cm="1">
+        <f t="array" ref="G396">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B396)*(curriculum!C:C=C396)*(curriculum!D:D=D396))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A397">
+        <v>396</v>
+      </c>
+      <c r="B397">
+        <v>2025</v>
+      </c>
+      <c r="C397">
+        <v>2</v>
+      </c>
+      <c r="D397" t="s">
+        <v>91</v>
+      </c>
+      <c r="E397">
+        <v>202100481</v>
+      </c>
+      <c r="F397" t="s">
+        <v>380</v>
+      </c>
+      <c r="G397" cm="1">
+        <f t="array" ref="G397">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B397)*(curriculum!C:C=C397)*(curriculum!D:D=D397))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A398">
+        <v>397</v>
+      </c>
+      <c r="B398">
+        <v>2025</v>
+      </c>
+      <c r="C398">
+        <v>2</v>
+      </c>
+      <c r="D398" t="s">
+        <v>91</v>
+      </c>
+      <c r="E398">
+        <v>202100638</v>
+      </c>
+      <c r="F398" t="s">
+        <v>289</v>
+      </c>
+      <c r="G398" cm="1">
+        <f t="array" ref="G398">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B398)*(curriculum!C:C=C398)*(curriculum!D:D=D398))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A399">
+        <v>398</v>
+      </c>
+      <c r="B399">
+        <v>2025</v>
+      </c>
+      <c r="C399">
+        <v>2</v>
+      </c>
+      <c r="D399" t="s">
+        <v>91</v>
+      </c>
+      <c r="E399">
+        <v>202100823</v>
+      </c>
+      <c r="F399" t="s">
+        <v>381</v>
+      </c>
+      <c r="G399" cm="1">
+        <f t="array" ref="G399">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B399)*(curriculum!C:C=C399)*(curriculum!D:D=D399))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A400">
+        <v>399</v>
+      </c>
+      <c r="B400">
+        <v>2025</v>
+      </c>
+      <c r="C400">
+        <v>2</v>
+      </c>
+      <c r="D400" t="s">
+        <v>91</v>
+      </c>
+      <c r="E400">
+        <v>202100899</v>
+      </c>
+      <c r="F400" t="s">
+        <v>382</v>
+      </c>
+      <c r="G400" cm="1">
+        <f t="array" ref="G400">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B400)*(curriculum!C:C=C400)*(curriculum!D:D=D400))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A401">
+        <v>400</v>
+      </c>
+      <c r="B401">
+        <v>2025</v>
+      </c>
+      <c r="C401">
+        <v>2</v>
+      </c>
+      <c r="D401" t="s">
+        <v>91</v>
+      </c>
+      <c r="E401">
+        <v>202101184</v>
+      </c>
+      <c r="F401" t="s">
+        <v>383</v>
+      </c>
+      <c r="G401" cm="1">
+        <f t="array" ref="G401">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B401)*(curriculum!C:C=C401)*(curriculum!D:D=D401))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A402">
+        <v>401</v>
+      </c>
+      <c r="B402">
+        <v>2025</v>
+      </c>
+      <c r="C402">
+        <v>2</v>
+      </c>
+      <c r="D402" t="s">
+        <v>91</v>
+      </c>
+      <c r="E402">
+        <v>202101962</v>
+      </c>
+      <c r="F402" t="s">
+        <v>343</v>
+      </c>
+      <c r="G402" cm="1">
+        <f t="array" ref="G402">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B402)*(curriculum!C:C=C402)*(curriculum!D:D=D402))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A403">
+        <v>402</v>
+      </c>
+      <c r="B403">
+        <v>2025</v>
+      </c>
+      <c r="C403">
+        <v>2</v>
+      </c>
+      <c r="D403" t="s">
+        <v>91</v>
+      </c>
+      <c r="E403">
+        <v>202102180</v>
+      </c>
+      <c r="F403" t="s">
+        <v>291</v>
+      </c>
+      <c r="G403" cm="1">
+        <f t="array" ref="G403">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B403)*(curriculum!C:C=C403)*(curriculum!D:D=D403))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A404">
+        <v>403</v>
+      </c>
+      <c r="B404">
+        <v>2025</v>
+      </c>
+      <c r="C404">
+        <v>2</v>
+      </c>
+      <c r="D404" t="s">
+        <v>91</v>
+      </c>
+      <c r="E404">
+        <v>202102627</v>
+      </c>
+      <c r="F404" t="s">
+        <v>384</v>
+      </c>
+      <c r="G404" cm="1">
+        <f t="array" ref="G404">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B404)*(curriculum!C:C=C404)*(curriculum!D:D=D404))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A405">
+        <v>404</v>
+      </c>
+      <c r="B405">
+        <v>2025</v>
+      </c>
+      <c r="C405">
+        <v>2</v>
+      </c>
+      <c r="D405" t="s">
+        <v>91</v>
+      </c>
+      <c r="E405">
+        <v>202103366</v>
+      </c>
+      <c r="F405" t="s">
+        <v>385</v>
+      </c>
+      <c r="G405" cm="1">
+        <f t="array" ref="G405">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B405)*(curriculum!C:C=C405)*(curriculum!D:D=D405))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A406">
+        <v>405</v>
+      </c>
+      <c r="B406">
+        <v>2025</v>
+      </c>
+      <c r="C406">
+        <v>2</v>
+      </c>
+      <c r="D406" t="s">
+        <v>91</v>
+      </c>
+      <c r="E406">
+        <v>202104582</v>
+      </c>
+      <c r="F406" t="s">
+        <v>386</v>
+      </c>
+      <c r="G406" cm="1">
+        <f t="array" ref="G406">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B406)*(curriculum!C:C=C406)*(curriculum!D:D=D406))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A407">
+        <v>406</v>
+      </c>
+      <c r="B407">
+        <v>2025</v>
+      </c>
+      <c r="C407">
+        <v>2</v>
+      </c>
+      <c r="D407" t="s">
+        <v>91</v>
+      </c>
+      <c r="E407">
+        <v>202200275</v>
+      </c>
+      <c r="F407" t="s">
+        <v>292</v>
+      </c>
+      <c r="G407" cm="1">
+        <f t="array" ref="G407">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B407)*(curriculum!C:C=C407)*(curriculum!D:D=D407))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A408">
+        <v>407</v>
+      </c>
+      <c r="B408">
+        <v>2025</v>
+      </c>
+      <c r="C408">
+        <v>2</v>
+      </c>
+      <c r="D408" t="s">
+        <v>91</v>
+      </c>
+      <c r="E408">
+        <v>202201078</v>
+      </c>
+      <c r="F408" t="s">
+        <v>293</v>
+      </c>
+      <c r="G408" cm="1">
+        <f t="array" ref="G408">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B408)*(curriculum!C:C=C408)*(curriculum!D:D=D408))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A409">
+        <v>408</v>
+      </c>
+      <c r="B409">
+        <v>2025</v>
+      </c>
+      <c r="C409">
+        <v>2</v>
+      </c>
+      <c r="D409" t="s">
+        <v>91</v>
+      </c>
+      <c r="E409">
+        <v>202201330</v>
+      </c>
+      <c r="F409" t="s">
+        <v>294</v>
+      </c>
+      <c r="G409" cm="1">
+        <f t="array" ref="G409">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B409)*(curriculum!C:C=C409)*(curriculum!D:D=D409))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A410">
+        <v>409</v>
+      </c>
+      <c r="B410">
+        <v>2025</v>
+      </c>
+      <c r="C410">
+        <v>2</v>
+      </c>
+      <c r="D410" t="s">
+        <v>91</v>
+      </c>
+      <c r="E410">
+        <v>202202007</v>
+      </c>
+      <c r="F410" t="s">
+        <v>387</v>
+      </c>
+      <c r="G410" cm="1">
+        <f t="array" ref="G410">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B410)*(curriculum!C:C=C410)*(curriculum!D:D=D410))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A411">
+        <v>410</v>
+      </c>
+      <c r="B411">
+        <v>2025</v>
+      </c>
+      <c r="C411">
+        <v>2</v>
+      </c>
+      <c r="D411" t="s">
+        <v>91</v>
+      </c>
+      <c r="E411">
+        <v>202202143</v>
+      </c>
+      <c r="F411" t="s">
+        <v>388</v>
+      </c>
+      <c r="G411" cm="1">
+        <f t="array" ref="G411">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B411)*(curriculum!C:C=C411)*(curriculum!D:D=D411))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A412">
+        <v>411</v>
+      </c>
+      <c r="B412">
+        <v>2025</v>
+      </c>
+      <c r="C412">
+        <v>2</v>
+      </c>
+      <c r="D412" t="s">
+        <v>91</v>
+      </c>
+      <c r="E412">
+        <v>202202771</v>
+      </c>
+      <c r="F412" t="s">
+        <v>389</v>
+      </c>
+      <c r="G412" cm="1">
+        <f t="array" ref="G412">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B412)*(curriculum!C:C=C412)*(curriculum!D:D=D412))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A413">
+        <v>412</v>
+      </c>
+      <c r="B413">
+        <v>2025</v>
+      </c>
+      <c r="C413">
+        <v>2</v>
+      </c>
+      <c r="D413" t="s">
+        <v>91</v>
+      </c>
+      <c r="E413">
+        <v>202203289</v>
+      </c>
+      <c r="F413" t="s">
+        <v>390</v>
+      </c>
+      <c r="G413" cm="1">
+        <f t="array" ref="G413">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B413)*(curriculum!C:C=C413)*(curriculum!D:D=D413))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A414">
+        <v>413</v>
+      </c>
+      <c r="B414">
+        <v>2025</v>
+      </c>
+      <c r="C414">
+        <v>2</v>
+      </c>
+      <c r="D414" t="s">
+        <v>91</v>
+      </c>
+      <c r="E414">
+        <v>202203662</v>
+      </c>
+      <c r="F414" t="s">
+        <v>391</v>
+      </c>
+      <c r="G414" cm="1">
+        <f t="array" ref="G414">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B414)*(curriculum!C:C=C414)*(curriculum!D:D=D414))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A415">
+        <v>414</v>
+      </c>
+      <c r="B415">
+        <v>2025</v>
+      </c>
+      <c r="C415">
+        <v>2</v>
+      </c>
+      <c r="D415" t="s">
+        <v>91</v>
+      </c>
+      <c r="E415">
+        <v>202204462</v>
+      </c>
+      <c r="F415" t="s">
+        <v>234</v>
+      </c>
+      <c r="G415" cm="1">
+        <f t="array" ref="G415">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B415)*(curriculum!C:C=C415)*(curriculum!D:D=D415))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A416">
+        <v>415</v>
+      </c>
+      <c r="B416">
+        <v>2025</v>
+      </c>
+      <c r="C416">
+        <v>2</v>
+      </c>
+      <c r="D416" t="s">
+        <v>91</v>
+      </c>
+      <c r="E416">
+        <v>202300403</v>
+      </c>
+      <c r="F416" t="s">
+        <v>392</v>
+      </c>
+      <c r="G416" cm="1">
+        <f t="array" ref="G416">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B416)*(curriculum!C:C=C416)*(curriculum!D:D=D416))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A417">
+        <v>416</v>
+      </c>
+      <c r="B417">
+        <v>2025</v>
+      </c>
+      <c r="C417">
+        <v>2</v>
+      </c>
+      <c r="D417" t="s">
+        <v>91</v>
+      </c>
+      <c r="E417">
+        <v>202300426</v>
+      </c>
+      <c r="F417" t="s">
+        <v>393</v>
+      </c>
+      <c r="G417" cm="1">
+        <f t="array" ref="G417">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B417)*(curriculum!C:C=C417)*(curriculum!D:D=D417))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A418">
+        <v>417</v>
+      </c>
+      <c r="B418">
+        <v>2025</v>
+      </c>
+      <c r="C418">
+        <v>2</v>
+      </c>
+      <c r="D418" t="s">
+        <v>91</v>
+      </c>
+      <c r="E418">
+        <v>202300799</v>
+      </c>
+      <c r="F418" t="s">
+        <v>298</v>
+      </c>
+      <c r="G418" cm="1">
+        <f t="array" ref="G418">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B418)*(curriculum!C:C=C418)*(curriculum!D:D=D418))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A419">
+        <v>418</v>
+      </c>
+      <c r="B419">
+        <v>2025</v>
+      </c>
+      <c r="C419">
+        <v>2</v>
+      </c>
+      <c r="D419" t="s">
+        <v>91</v>
+      </c>
+      <c r="E419">
+        <v>202302478</v>
+      </c>
+      <c r="F419" t="s">
+        <v>349</v>
+      </c>
+      <c r="G419" cm="1">
+        <f t="array" ref="G419">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B419)*(curriculum!C:C=C419)*(curriculum!D:D=D419))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A420">
+        <v>419</v>
+      </c>
+      <c r="B420">
+        <v>2025</v>
+      </c>
+      <c r="C420">
+        <v>2</v>
+      </c>
+      <c r="D420" t="s">
+        <v>91</v>
+      </c>
+      <c r="E420">
+        <v>202303253</v>
+      </c>
+      <c r="F420" t="s">
+        <v>350</v>
+      </c>
+      <c r="G420" cm="1">
+        <f t="array" ref="G420">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B420)*(curriculum!C:C=C420)*(curriculum!D:D=D420))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A421">
+        <v>420</v>
+      </c>
+      <c r="B421">
+        <v>2025</v>
+      </c>
+      <c r="C421">
+        <v>2</v>
+      </c>
+      <c r="D421" t="s">
+        <v>91</v>
+      </c>
+      <c r="E421">
+        <v>202303636</v>
+      </c>
+      <c r="F421" t="s">
+        <v>304</v>
+      </c>
+      <c r="G421" cm="1">
+        <f t="array" ref="G421">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B421)*(curriculum!C:C=C421)*(curriculum!D:D=D421))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A422">
+        <v>421</v>
+      </c>
+      <c r="B422">
+        <v>2025</v>
+      </c>
+      <c r="C422">
+        <v>2</v>
+      </c>
+      <c r="D422" t="s">
+        <v>91</v>
+      </c>
+      <c r="E422" s="1">
+        <v>202303694</v>
+      </c>
+      <c r="F422" t="s">
+        <v>278</v>
+      </c>
+      <c r="G422" cm="1">
+        <f t="array" ref="G422">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B422)*(curriculum!C:C=C422)*(curriculum!D:D=D422))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A423">
+        <v>422</v>
+      </c>
+      <c r="B423">
+        <v>2025</v>
+      </c>
+      <c r="C423">
+        <v>2</v>
+      </c>
+      <c r="D423" t="s">
+        <v>91</v>
+      </c>
+      <c r="E423" s="1">
+        <v>202304467</v>
+      </c>
+      <c r="F423" t="s">
+        <v>354</v>
+      </c>
+      <c r="G423" cm="1">
+        <f t="array" ref="G423">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B423)*(curriculum!C:C=C423)*(curriculum!D:D=D423))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A424">
+        <v>423</v>
+      </c>
+      <c r="B424">
+        <v>2025</v>
+      </c>
+      <c r="C424">
+        <v>2</v>
+      </c>
+      <c r="D424" t="s">
+        <v>91</v>
+      </c>
+      <c r="E424" s="1">
+        <v>202304644</v>
+      </c>
+      <c r="F424" t="s">
+        <v>305</v>
+      </c>
+      <c r="G424" cm="1">
+        <f t="array" ref="G424">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B424)*(curriculum!C:C=C424)*(curriculum!D:D=D424))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A425">
+        <v>424</v>
+      </c>
+      <c r="B425">
+        <v>2025</v>
+      </c>
+      <c r="C425">
+        <v>2</v>
+      </c>
+      <c r="D425" t="s">
+        <v>91</v>
+      </c>
+      <c r="E425" s="1">
+        <v>202400305</v>
+      </c>
+      <c r="F425" t="s">
+        <v>394</v>
+      </c>
+      <c r="G425" cm="1">
+        <f t="array" ref="G425">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B425)*(curriculum!C:C=C425)*(curriculum!D:D=D425))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A426">
+        <v>425</v>
+      </c>
+      <c r="B426">
+        <v>2025</v>
+      </c>
+      <c r="C426">
+        <v>2</v>
+      </c>
+      <c r="D426" t="s">
+        <v>91</v>
+      </c>
+      <c r="E426" s="1">
+        <v>202400473</v>
+      </c>
+      <c r="F426" t="s">
+        <v>395</v>
+      </c>
+      <c r="G426" cm="1">
+        <f t="array" ref="G426">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B426)*(curriculum!C:C=C426)*(curriculum!D:D=D426))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A427">
+        <v>426</v>
+      </c>
+      <c r="B427">
+        <v>2025</v>
+      </c>
+      <c r="C427">
+        <v>2</v>
+      </c>
+      <c r="D427" t="s">
+        <v>91</v>
+      </c>
+      <c r="E427" s="1">
+        <v>202401153</v>
+      </c>
+      <c r="F427" t="s">
+        <v>314</v>
+      </c>
+      <c r="G427" cm="1">
+        <f t="array" ref="G427">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B427)*(curriculum!C:C=C427)*(curriculum!D:D=D427))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A428">
+        <v>427</v>
+      </c>
+      <c r="B428">
+        <v>2025</v>
+      </c>
+      <c r="C428">
+        <v>2</v>
+      </c>
+      <c r="D428" t="s">
+        <v>91</v>
+      </c>
+      <c r="E428" s="1">
+        <v>202401947</v>
+      </c>
+      <c r="F428" t="s">
+        <v>316</v>
+      </c>
+      <c r="G428" cm="1">
+        <f t="array" ref="G428">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B428)*(curriculum!C:C=C428)*(curriculum!D:D=D428))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A429">
+        <v>428</v>
+      </c>
+      <c r="B429">
+        <v>2025</v>
+      </c>
+      <c r="C429">
+        <v>2</v>
+      </c>
+      <c r="D429" t="s">
+        <v>91</v>
+      </c>
+      <c r="E429" s="1">
+        <v>202402469</v>
+      </c>
+      <c r="F429" t="s">
+        <v>396</v>
+      </c>
+      <c r="G429" cm="1">
+        <f t="array" ref="G429">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B429)*(curriculum!C:C=C429)*(curriculum!D:D=D429))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A430">
+        <v>429</v>
+      </c>
+      <c r="B430">
+        <v>2025</v>
+      </c>
+      <c r="C430">
+        <v>2</v>
+      </c>
+      <c r="D430" t="s">
+        <v>91</v>
+      </c>
+      <c r="E430" s="1">
+        <v>202402954</v>
+      </c>
+      <c r="F430" t="s">
+        <v>322</v>
+      </c>
+      <c r="G430" cm="1">
+        <f t="array" ref="G430">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B430)*(curriculum!C:C=C430)*(curriculum!D:D=D430))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A431">
+        <v>430</v>
+      </c>
+      <c r="B431">
+        <v>2025</v>
+      </c>
+      <c r="C431">
+        <v>2</v>
+      </c>
+      <c r="D431" t="s">
+        <v>91</v>
+      </c>
+      <c r="E431" s="1">
+        <v>202403302</v>
+      </c>
+      <c r="F431" t="s">
+        <v>326</v>
+      </c>
+      <c r="G431" cm="1">
+        <f t="array" ref="G431">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B431)*(curriculum!C:C=C431)*(curriculum!D:D=D431))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A432">
+        <v>431</v>
+      </c>
+      <c r="B432">
+        <v>2025</v>
+      </c>
+      <c r="C432">
+        <v>2</v>
+      </c>
+      <c r="D432" t="s">
+        <v>91</v>
+      </c>
+      <c r="E432" s="1">
+        <v>202403870</v>
+      </c>
+      <c r="F432" t="s">
+        <v>328</v>
+      </c>
+      <c r="G432" cm="1">
+        <f t="array" ref="G432">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B432)*(curriculum!C:C=C432)*(curriculum!D:D=D432))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A433">
+        <v>432</v>
+      </c>
+      <c r="B433">
+        <v>2025</v>
+      </c>
+      <c r="C433">
+        <v>2</v>
+      </c>
+      <c r="D433" t="s">
+        <v>91</v>
+      </c>
+      <c r="E433" s="1">
+        <v>202403912</v>
+      </c>
+      <c r="F433" t="s">
+        <v>329</v>
+      </c>
+      <c r="G433" cm="1">
+        <f t="array" ref="G433">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B433)*(curriculum!C:C=C433)*(curriculum!D:D=D433))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A434">
+        <v>433</v>
+      </c>
+      <c r="B434">
+        <v>2025</v>
+      </c>
+      <c r="C434">
+        <v>2</v>
+      </c>
+      <c r="D434" t="s">
+        <v>91</v>
+      </c>
+      <c r="E434" s="1">
+        <v>202404225</v>
+      </c>
+      <c r="F434" t="s">
+        <v>397</v>
+      </c>
+      <c r="G434" cm="1">
+        <f t="array" ref="G434">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B434)*(curriculum!C:C=C434)*(curriculum!D:D=D434))</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A435">
+        <v>434</v>
+      </c>
+      <c r="B435">
+        <v>2025</v>
+      </c>
+      <c r="C435">
+        <v>2</v>
+      </c>
+      <c r="D435" t="s">
+        <v>91</v>
+      </c>
+      <c r="E435" s="1">
+        <v>202583014</v>
+      </c>
+      <c r="F435" t="s">
+        <v>398</v>
+      </c>
+      <c r="G435" cm="1">
+        <f t="array" ref="G435">_xlfn._xlws.FILTER(curriculum!A:A,(curriculum!B:B=B435)*(curriculum!C:C=C435)*(curriculum!D:D=D435))</f>
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G373">

</xml_diff>